<commit_message>
accepted + rejected columns correct
</commit_message>
<xml_diff>
--- a/mm1_as_servers1_tweaked/runs_data_ram_70.xlsx
+++ b/mm1_as_servers1_tweaked/runs_data_ram_70.xlsx
@@ -77,13 +77,41 @@
           <t>number of servers</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>accepted</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>rejected</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>61.43229166666667</v>
+        <v>76.55989583333334</v>
       </c>
       <c r="B2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>435.0</v>
+      </c>
+      <c r="D2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>77.22916666666666</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>402.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>438.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>